<commit_message>
[ll] commit before beginning code for respin
</commit_message>
<xml_diff>
--- a/board/span-ion-cfd/BoM.xlsx
+++ b/board/span-ion-cfd/BoM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4830" windowHeight="2340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14970" windowHeight="3390"/>
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="82">
   <si>
     <t>Comment</t>
   </si>
@@ -71,7 +71,7 @@
     <t>10nF</t>
   </si>
   <si>
-    <t>C4, C5, C6, C7, C10, C11, C12, C16, C17, C18, C20, C21, C22, C30, C31, C32, C33</t>
+    <t>C4, C5, C6, C7, C10, C11, C12, C16, C17, C18, C20, C21, C22, C30</t>
   </si>
   <si>
     <t>(10nF)</t>
@@ -80,31 +80,37 @@
     <t>C25, C26, C27, C28, C29</t>
   </si>
   <si>
-    <t>C34</t>
-  </si>
-  <si>
-    <t>C35</t>
-  </si>
-  <si>
-    <t>C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46, C47, C48, C49, C50, C51, C52, C53, C54, C55, C56</t>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>C32, C33, C34, C35, C36, C37, C38, C39, C40, C41, C42, C43, C44, C45, C46, C47, C48, C49, C50, C51, C52</t>
   </si>
   <si>
     <t>CFD_package</t>
   </si>
   <si>
-    <t>CFD_PACKAGE1</t>
+    <t>CFD</t>
   </si>
   <si>
     <t>QFN50P700X700X80_HS-45N_WIDEVIAS</t>
   </si>
   <si>
+    <t>Corner Mount</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
+    <t>CORNER1, CORNER2, CORNER3, CORNER4</t>
+  </si>
+  <si>
+    <t>CornerMount</t>
+  </si>
+  <si>
     <t>Zener Voltage Regulator, 2-Pin SOD-123, Pb-Free, Tape and Reel</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8</t>
+    <t>D1, D2</t>
   </si>
   <si>
     <t>ONSC-SOD-123-2-425-04_V</t>
@@ -152,7 +158,7 @@
     <t>SMA Connector, Pitch 5.08 mm, 1 Position, Height 9.5 mm, Tail Length 4 mm, -65 to 165 degC, RoHS, Bulk</t>
   </si>
   <si>
-    <t>J1</t>
+    <t>J1, J2, J3, J4, J5, J6</t>
   </si>
   <si>
     <t>TECO-5-1814832-1_V</t>
@@ -167,34 +173,37 @@
     <t>Header, 2-Pin</t>
   </si>
   <si>
-    <t>P1, P2, P3, P4, P5, P6, P7, P8, P9, P12, P13, P14, P15, P18, P19, P20, P21, P22, P23, P24, P25, P26, P27, P28, P29, P30, P31</t>
+    <t>P1, P2, P3, P4, P5, P6, P7, P8, P9, P12, P13, P14, P15, P16, P17, P18, P19, P20, P21, P22, P23, P24, P25, P26, P27, P28</t>
   </si>
   <si>
     <t>HDR1X2</t>
   </si>
   <si>
-    <t>BFR182W</t>
-  </si>
-  <si>
-    <t>NPN Silicon RF Transistor, 12 V VCEO, 35 mA IC, 19 dB Gmax, SOT323, Green</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>INF-SOT323_L</t>
-  </si>
-  <si>
-    <t>CMP-1191-00013-1</t>
-  </si>
-  <si>
-    <t>0Ohm</t>
-  </si>
-  <si>
-    <t>Chip Resistor, 0 Ohm, Jumper, 100 mW, -55 to 155 degC, 0603 (1608 Metric), RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4</t>
+    <t>Header 24</t>
+  </si>
+  <si>
+    <t>Header, 24-Pin</t>
+  </si>
+  <si>
+    <t>P10, P11</t>
+  </si>
+  <si>
+    <t>HDR1X24</t>
+  </si>
+  <si>
+    <t>Header 1</t>
+  </si>
+  <si>
+    <t>P29, P30, P31, P32</t>
+  </si>
+  <si>
+    <t>Header1</t>
+  </si>
+  <si>
+    <t>(&lt;50Ohm)</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
   </si>
   <si>
     <t>RESC1609X50X30NL8T20</t>
@@ -203,16 +212,16 @@
     <t>CMP-2000-03816-5</t>
   </si>
   <si>
-    <t>R5</t>
+    <t>(0/50Ohm)</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
   <si>
     <t>(50Ohm)</t>
   </si>
   <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R7</t>
+    <t>R4, R5, R6, R7, R8</t>
   </si>
   <si>
     <t>TEENSY_3.5/3.6</t>
@@ -236,16 +245,34 @@
     <t>CMP-0394-00378-2</t>
   </si>
   <si>
+    <t>Container No.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>Do Not Populate</t>
   </si>
   <si>
-    <t>2x Header 24</t>
-  </si>
-  <si>
-    <t>Container No.</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>2pF</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>TI site maintenance</t>
+  </si>
+  <si>
+    <t>Mouser cart</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Digikey cart</t>
+  </si>
+  <si>
+    <t>Out of stock</t>
   </si>
 </sst>
 </file>
@@ -302,24 +329,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,21 +615,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="106.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="3" max="3" width="76.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -633,11 +651,14 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -656,11 +677,12 @@
       <c r="F2" s="1">
         <v>5</v>
       </c>
-      <c r="G2" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -679,11 +701,12 @@
       <c r="F3" s="1">
         <v>6</v>
       </c>
-      <c r="G3" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -700,13 +723,14 @@
         <v>10</v>
       </c>
       <c r="F4" s="1">
-        <v>17</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -725,13 +749,14 @@
       <c r="F5" s="1">
         <v>5</v>
       </c>
-      <c r="G5" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -748,11 +773,14 @@
       <c r="F6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -767,217 +795,231 @@
         <v>10</v>
       </c>
       <c r="F7" s="1">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1">
-        <v>21</v>
-      </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="F11" s="1">
         <v>2</v>
       </c>
-      <c r="G11" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
-      <c r="G12" s="7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
       </c>
-      <c r="G13" s="7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="F15" s="1">
-        <v>27</v>
-      </c>
-      <c r="G15" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="7">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>55</v>
@@ -986,126 +1028,132 @@
         <v>56</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F17" s="1">
         <v>4</v>
       </c>
-      <c r="G17" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="G19" s="7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
       </c>
-      <c r="G21" s="7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F22" s="1">
         <v>7</v>
       </c>
-      <c r="G22" s="7">
-        <v>15</v>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>